<commit_message>
fixed errors in para names for lumbar s
</commit_message>
<xml_diff>
--- a/src/main/resources/rulesConfiguration/rule specifications.xlsx
+++ b/src/main/resources/rulesConfiguration/rule specifications.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17571"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17766"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\code\dva-sop-api\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\code\dva-sop-api\src\main\resources\rulesConfiguration\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <workbookProtection lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18000" windowHeight="23880"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18000" windowHeight="23880" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="RH" sheetId="1" r:id="rId1"/>
@@ -89,9 +89,6 @@
     <t>F2014L00930</t>
   </si>
   <si>
-    <t>6(j), 6(x)</t>
-  </si>
-  <si>
     <t>thoracric spondylosis</t>
   </si>
   <si>
@@ -113,9 +110,6 @@
     <t>F2011C00491</t>
   </si>
   <si>
-    <t>6(m)(i),6(gg)(i)</t>
-  </si>
-  <si>
     <t>F2011C00492</t>
   </si>
   <si>
@@ -123,6 +117,12 @@
   </si>
   <si>
     <t>Royal Australian Air Force</t>
+  </si>
+  <si>
+    <t>6(i), 6(x)</t>
+  </si>
+  <si>
+    <t>6(m)(i),6(ff)(i)</t>
   </si>
 </sst>
 </file>
@@ -181,9 +181,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="5">
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -256,6 +253,9 @@
         <scheme val="minor"/>
       </font>
     </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -289,14 +289,14 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:H13" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:H13" totalsRowShown="0" headerRowDxfId="4">
   <autoFilter ref="A1:H13"/>
   <tableColumns count="8">
     <tableColumn id="1" name="Condition"/>
-    <tableColumn id="2" name="Instrument ID" dataDxfId="4"/>
-    <tableColumn id="3" name="Factor References" dataDxfId="3"/>
-    <tableColumn id="4" name="Service Branch" dataDxfId="2"/>
-    <tableColumn id="5" name="Rank" dataDxfId="1"/>
+    <tableColumn id="2" name="Instrument ID" dataDxfId="3"/>
+    <tableColumn id="3" name="Factor References" dataDxfId="2"/>
+    <tableColumn id="4" name="Service Branch" dataDxfId="1"/>
+    <tableColumn id="5" name="Rank" dataDxfId="0"/>
     <tableColumn id="6" name="CFTS weeks"/>
     <tableColumn id="7" name="Accumulation Rate per week"/>
     <tableColumn id="8" name="Accumulation Unit"/>
@@ -604,8 +604,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -852,13 +852,13 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="C8" t="s">
         <v>22</v>
-      </c>
-      <c r="C8" t="s">
-        <v>23</v>
       </c>
       <c r="D8" t="s">
         <v>16</v>
@@ -878,13 +878,13 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="C9" t="s">
         <v>22</v>
-      </c>
-      <c r="C9" t="s">
-        <v>23</v>
       </c>
       <c r="D9" t="s">
         <v>16</v>
@@ -904,13 +904,13 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="C10" t="s">
         <v>22</v>
-      </c>
-      <c r="C10" t="s">
-        <v>23</v>
       </c>
       <c r="D10" t="s">
         <v>16</v>
@@ -930,13 +930,13 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="C11" t="s">
         <v>22</v>
-      </c>
-      <c r="C11" t="s">
-        <v>23</v>
       </c>
       <c r="D11" t="s">
         <v>17</v>
@@ -956,13 +956,13 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="C12" t="s">
         <v>22</v>
-      </c>
-      <c r="C12" t="s">
-        <v>23</v>
       </c>
       <c r="D12" t="s">
         <v>17</v>
@@ -982,13 +982,13 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" t="s">
         <v>26</v>
       </c>
-      <c r="B13" t="s">
-        <v>27</v>
-      </c>
       <c r="C13" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D13" t="s">
         <v>16</v>
@@ -1014,13 +1014,13 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" t="s">
         <v>26</v>
       </c>
-      <c r="B14" t="s">
-        <v>27</v>
-      </c>
       <c r="C14" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D14" t="s">
         <v>16</v>
@@ -1046,13 +1046,13 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" t="s">
         <v>26</v>
       </c>
-      <c r="B15" t="s">
-        <v>27</v>
-      </c>
       <c r="C15" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D15" t="s">
         <v>16</v>
@@ -1078,13 +1078,13 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" t="s">
         <v>26</v>
       </c>
-      <c r="B16" t="s">
-        <v>27</v>
-      </c>
       <c r="C16" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D16" t="s">
         <v>17</v>
@@ -1104,13 +1104,13 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" t="s">
         <v>26</v>
       </c>
-      <c r="B17" t="s">
-        <v>27</v>
-      </c>
       <c r="C17" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D17" t="s">
         <v>17</v>
@@ -1130,13 +1130,13 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" t="s">
         <v>26</v>
       </c>
-      <c r="B18" t="s">
-        <v>27</v>
-      </c>
       <c r="C18" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D18" t="s">
         <v>17</v>
@@ -1200,8 +1200,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1250,7 +1250,7 @@
         <v>19</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D2" t="s">
         <v>16</v>
@@ -1276,7 +1276,7 @@
         <v>19</v>
       </c>
       <c r="C3" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D3" t="s">
         <v>16</v>
@@ -1302,7 +1302,7 @@
         <v>19</v>
       </c>
       <c r="C4" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D4" t="s">
         <v>16</v>
@@ -1328,7 +1328,7 @@
         <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D5" t="s">
         <v>17</v>
@@ -1348,13 +1348,13 @@
     </row>
     <row r="6" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>25</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>16</v>
@@ -1374,13 +1374,13 @@
     </row>
     <row r="7" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>25</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>16</v>
@@ -1400,13 +1400,13 @@
     </row>
     <row r="8" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>25</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>16</v>
@@ -1426,13 +1426,13 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>25</v>
       </c>
       <c r="D9" t="s">
         <v>17</v>
@@ -1452,13 +1452,13 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>16</v>
@@ -1478,13 +1478,13 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>16</v>
@@ -1504,13 +1504,13 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>16</v>
@@ -1530,13 +1530,13 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>17</v>
@@ -1618,7 +1618,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B3" t="s">
         <v>18</v>

</xml_diff>